<commit_message>
Made some changes in file lekovi
</commit_message>
<xml_diff>
--- a/data-set/lekovi.xlsx
+++ b/data-set/lekovi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maga\Desktop\ProjekatIZ\InzenjeringZnanja\data-set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7498A6-321D-481A-AAD0-65D31AE6E189}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C139EEB8-8EEE-4FD8-B145-A134E1782F11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2820" yWindow="2610" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>#id,listaTerapija</t>
   </si>
   <si>
-    <t>1;aperol</t>
+    <t>1;nitroglicerin,aspirin,atenolol,propranolol,rosuvastatin</t>
+  </si>
+  <si>
+    <t>2;aspirin, nitroglicerin, propranolol</t>
   </si>
 </sst>
 </file>
@@ -348,10 +351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -366,6 +369,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>